<commit_message>
testing  increase of demand by 2
</commit_message>
<xml_diff>
--- a/data/exported_toward_bb_2050.xlsx
+++ b/data/exported_toward_bb_2050.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76161B21-E405-498F-AC90-53EB7F222827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A1AD7D-67B2-4BB4-A84B-70077BCB4DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -634,7 +634,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -656,6 +656,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,7 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -698,6 +704,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8715,8 +8722,8 @@
   </sheetPr>
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8869,16 +8876,16 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="9">
         <v>2</v>
       </c>
       <c r="F11" s="8"/>
@@ -9516,16 +9523,16 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D55" s="9">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
no increase in demand
</commit_message>
<xml_diff>
--- a/data/exported_toward_bb_2050.xlsx
+++ b/data/exported_toward_bb_2050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A1AD7D-67B2-4BB4-A84B-70077BCB4DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454152E3-EB4A-496C-B20B-163834E28D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28815" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grid" sheetId="1" r:id="rId1"/>
@@ -8722,8 +8722,8 @@
   </sheetPr>
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8886,7 +8886,7 @@
         <v>101</v>
       </c>
       <c r="D11" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>

</xml_diff>